<commit_message>
CIERRE 27 FEB 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #01   ENERO 2023/CREDITOS     ZAVALETA  ENERO 2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #01   ENERO 2023/CREDITOS     ZAVALETA  ENERO 2023.xlsx
@@ -2687,7 +2687,7 @@
   <dimension ref="A2:Z61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2756,7 +2756,7 @@
       <c r="I4" s="88"/>
       <c r="J4" s="20">
         <f>E47+I4</f>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -2778,7 +2778,7 @@
       <c r="I5" s="88"/>
       <c r="J5" s="20">
         <f>J4+I5</f>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
       <c r="I6" s="88"/>
       <c r="J6" s="20">
         <f t="shared" ref="J6:J29" si="1">J5+I6</f>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
       <c r="I7" s="88"/>
       <c r="J7" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
       <c r="I8" s="88"/>
       <c r="J8" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
       <c r="I9" s="84"/>
       <c r="J9" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
       <c r="I10" s="84"/>
       <c r="J10" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
@@ -2912,7 +2912,7 @@
       <c r="I11" s="84"/>
       <c r="J11" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
@@ -2934,151 +2934,205 @@
       <c r="I12" s="84"/>
       <c r="J12" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="21"/>
+      <c r="B13" s="91">
+        <v>44970</v>
+      </c>
+      <c r="C13" s="92">
+        <v>44977</v>
+      </c>
+      <c r="D13" s="21">
+        <v>15000</v>
+      </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>341804</v>
       </c>
       <c r="G13" s="82"/>
       <c r="H13" s="90"/>
       <c r="I13" s="84"/>
       <c r="J13" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="91"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="21"/>
+      <c r="B14" s="91">
+        <v>44973</v>
+      </c>
+      <c r="C14" s="92">
+        <v>44977</v>
+      </c>
+      <c r="D14" s="21">
+        <v>25683.5</v>
+      </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>367487.5</v>
       </c>
       <c r="G14" s="82"/>
       <c r="H14" s="90"/>
       <c r="I14" s="84"/>
       <c r="J14" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="91"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="21"/>
+      <c r="B15" s="91">
+        <v>44974</v>
+      </c>
+      <c r="C15" s="92">
+        <v>44977</v>
+      </c>
+      <c r="D15" s="21">
+        <v>45894</v>
+      </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>413381.5</v>
       </c>
       <c r="G15" s="82"/>
       <c r="H15" s="90"/>
       <c r="I15" s="84"/>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="21"/>
+      <c r="B16" s="91">
+        <v>44975</v>
+      </c>
+      <c r="C16" s="92">
+        <v>44977</v>
+      </c>
+      <c r="D16" s="21">
+        <v>42408.5</v>
+      </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>455790</v>
       </c>
       <c r="G16" s="82"/>
       <c r="H16" s="90"/>
       <c r="I16" s="84"/>
       <c r="J16" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="91">
+        <v>44976</v>
+      </c>
+      <c r="C17" s="92">
+        <v>44982</v>
+      </c>
+      <c r="D17" s="21">
+        <v>60371</v>
+      </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>516161</v>
       </c>
       <c r="G17" s="82"/>
       <c r="H17" s="87"/>
       <c r="I17" s="84"/>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="91"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="21"/>
+      <c r="B18" s="91">
+        <v>44977</v>
+      </c>
+      <c r="C18" s="92">
+        <v>44982</v>
+      </c>
+      <c r="D18" s="21">
+        <v>36667.5</v>
+      </c>
       <c r="E18" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>552828.5</v>
       </c>
       <c r="G18" s="82"/>
       <c r="H18" s="87"/>
       <c r="I18" s="84"/>
       <c r="J18" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="91">
+        <v>44978</v>
+      </c>
+      <c r="C19" s="92">
+        <v>44982</v>
+      </c>
+      <c r="D19" s="21">
+        <v>37369.5</v>
+      </c>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>590198</v>
       </c>
       <c r="G19" s="82"/>
       <c r="H19" s="87"/>
       <c r="I19" s="84"/>
       <c r="J19" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="91"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="91">
+        <v>44979</v>
+      </c>
+      <c r="C20" s="92">
+        <v>44982</v>
+      </c>
+      <c r="D20" s="21">
+        <v>40263</v>
+      </c>
       <c r="E20" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>630461</v>
       </c>
       <c r="G20" s="82"/>
       <c r="H20" s="87"/>
       <c r="I20" s="88"/>
       <c r="J20" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="91"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="91">
+        <v>44980</v>
+      </c>
+      <c r="C21" s="92">
+        <v>44982</v>
+      </c>
+      <c r="D21" s="21">
+        <v>78783</v>
+      </c>
       <c r="E21" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G21" s="82"/>
       <c r="H21" s="87"/>
       <c r="I21" s="88"/>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -3087,14 +3141,14 @@
       <c r="D22" s="21"/>
       <c r="E22" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="87"/>
       <c r="I22" s="88"/>
       <c r="J22" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -3103,14 +3157,14 @@
       <c r="D23" s="21"/>
       <c r="E23" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G23" s="82"/>
       <c r="H23" s="87"/>
       <c r="I23" s="88"/>
       <c r="J23" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -3119,14 +3173,14 @@
       <c r="D24" s="21"/>
       <c r="E24" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G24" s="82"/>
       <c r="H24" s="87"/>
       <c r="I24" s="88"/>
       <c r="J24" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -3135,14 +3189,14 @@
       <c r="D25" s="21"/>
       <c r="E25" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G25" s="82"/>
       <c r="H25" s="87"/>
       <c r="I25" s="93"/>
       <c r="J25" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -3151,14 +3205,14 @@
       <c r="D26" s="21"/>
       <c r="E26" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G26" s="82"/>
       <c r="H26" s="87"/>
       <c r="I26" s="93"/>
       <c r="J26" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3167,14 +3221,14 @@
       <c r="D27" s="21"/>
       <c r="E27" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G27" s="94"/>
       <c r="H27" s="95"/>
       <c r="I27" s="96"/>
       <c r="J27" s="20">
         <f t="shared" si="1"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -3183,7 +3237,7 @@
       <c r="D28" s="21"/>
       <c r="E28" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="F28" s="97"/>
       <c r="G28" s="98">
@@ -3197,7 +3251,7 @@
       </c>
       <c r="J28" s="20">
         <f t="shared" si="1"/>
-        <v>-1702537.58</v>
+        <v>-1320097.58</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
@@ -3206,14 +3260,14 @@
       <c r="D29" s="21"/>
       <c r="E29" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G29" s="99"/>
       <c r="H29" s="99"/>
       <c r="I29" s="99"/>
       <c r="J29" s="20">
         <f t="shared" si="1"/>
-        <v>-1702537.58</v>
+        <v>-1320097.58</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
@@ -3222,7 +3276,7 @@
       <c r="D30" s="21"/>
       <c r="E30" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G30" s="99"/>
       <c r="H30" s="99"/>
@@ -3235,7 +3289,7 @@
       <c r="D31" s="102"/>
       <c r="E31" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="G31" s="99"/>
       <c r="H31" s="99"/>
@@ -3248,7 +3302,7 @@
       <c r="D32" s="103"/>
       <c r="E32" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15" x14ac:dyDescent="0.25">
@@ -3257,7 +3311,7 @@
       <c r="D33" s="103"/>
       <c r="E33" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15" x14ac:dyDescent="0.25">
@@ -3266,7 +3320,7 @@
       <c r="D34" s="103"/>
       <c r="E34" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -3275,7 +3329,7 @@
       <c r="D35" s="84"/>
       <c r="E35" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -3284,7 +3338,7 @@
       <c r="D36" s="84"/>
       <c r="E36" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -3293,7 +3347,7 @@
       <c r="D37" s="84"/>
       <c r="E37" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -3302,7 +3356,7 @@
       <c r="D38" s="84"/>
       <c r="E38" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -3311,7 +3365,7 @@
       <c r="D39" s="84"/>
       <c r="E39" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -3320,7 +3374,7 @@
       <c r="D40" s="84"/>
       <c r="E40" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -3329,7 +3383,7 @@
       <c r="D41" s="84"/>
       <c r="E41" s="104">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -3338,7 +3392,7 @@
       <c r="D42" s="84"/>
       <c r="E42" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -3347,7 +3401,7 @@
       <c r="D43" s="84"/>
       <c r="E43" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -3356,7 +3410,7 @@
       <c r="D44" s="84"/>
       <c r="E44" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -3365,7 +3419,7 @@
       <c r="D45" s="84"/>
       <c r="E45" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -3374,7 +3428,7 @@
       <c r="D46" s="84"/>
       <c r="E46" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="F46"/>
     </row>
@@ -3384,7 +3438,7 @@
       <c r="D47" s="84"/>
       <c r="E47" s="20">
         <f t="shared" si="0"/>
-        <v>326804</v>
+        <v>709244</v>
       </c>
       <c r="F47"/>
     </row>

</xml_diff>